<commit_message>
Provide default gramcat when importing variation
</commit_message>
<xml_diff>
--- a/tests/fixtures/variation-missing-gramcat.xlsx
+++ b/tests/fixtures/variation-missing-gramcat.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t xml:space="preserve">abanico</t>
   </si>
@@ -35,12 +35,6 @@
   </si>
   <si>
     <t xml:space="preserve">cuairón</t>
-  </si>
-  <si>
-    <t xml:space="preserve">azar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wrong.</t>
   </si>
 </sst>
 </file>
@@ -137,10 +131,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -167,17 +161,6 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>5</v>
-      </c>
-    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>